<commit_message>
Changes of Audit history
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="102">
   <si>
     <t>Service</t>
   </si>
@@ -291,6 +291,89 @@
   </si>
   <si>
     <t>151874761</t>
+  </si>
+  <si>
+    <t>14699021</t>
+  </si>
+  <si>
+    <t>14699028</t>
+  </si>
+  <si>
+    <t>14699039</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.isDisplayed()" because "element" is null</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=117.0.5938.149)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.149, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:55020}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: dd5ca1e3166381a142b92c679b7fff0c
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to be clickable: By.id: idJobOverview (tried for 60 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>14699099</t>
+  </si>
+  <si>
+    <t>14699102</t>
+  </si>
+  <si>
+    <t>14699105</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=117.0.5938.149)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.149, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62539}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a81fe3c30db9708ab561155812cad2df
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>14699123</t>
+  </si>
+  <si>
+    <t>RT00005906</t>
+  </si>
+  <si>
+    <t>152472050</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#aNGLLogo"}
+  (Session info: headless chrome=117.0.5938.149)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.149, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62539}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a81fe3c30db9708ab561155812cad2df
+*** Element info: {Using=id, value=aNGLLogo}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=117.0.5938.149)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 117.0.5938.149, chrome: {chromedriverVersion: 117.0.5938.149 (e3344ddefa1..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62631}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 42f4784c24abe7aa08ca6b796ec528f6
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>14699197</t>
+  </si>
+  <si>
+    <t>14699198</t>
   </si>
 </sst>
 </file>
@@ -695,7 +778,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
@@ -745,7 +828,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -763,7 +846,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -907,7 +990,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -943,11 +1026,11 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
         <v>39</v>
@@ -961,11 +1044,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>39</v>
@@ -1019,7 +1102,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -1037,10 +1120,10 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F18" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1055,7 +1138,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F19" t="s">
         <v>39</v>
@@ -1072,7 +1155,7 @@
       </c>
       <c r="D20" s="1"/>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -1142,7 +1225,7 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -1180,7 +1263,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F26" t="s">
         <v>39</v>
@@ -1193,10 +1276,10 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s">
         <v>39</v>
@@ -1207,10 +1290,10 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F28" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Changes of NA OCP
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="144">
   <si>
     <t>Service</t>
   </si>
@@ -455,6 +455,72 @@
   </si>
   <si>
     <t>156139881</t>
+  </si>
+  <si>
+    <t>15114894</t>
+  </si>
+  <si>
+    <t>15114934</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to no longer be visible: By.xpath: //*[@class='ajax-loadernew'] (tried for 7 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.8', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.85, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50850}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 10573221fe6af0f09ad1c5ed7a45ad53</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.85)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.8', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.85, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50850}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 10573221fe6af0f09ad1c5ed7a45ad53
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>15115072</t>
+  </si>
+  <si>
+    <t>15115109</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.clear()" because the return value of "connect_OCBaseMethods.OrderCreation.isElementPresent(String)" is null</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.85)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.8', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.85, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:56096}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: bb3b8de3a260aa3e5dcc34dea974598d
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>15115182</t>
+  </si>
+  <si>
+    <t>15115215</t>
+  </si>
+  <si>
+    <t>15115228</t>
+  </si>
+  <si>
+    <t>15115233</t>
+  </si>
+  <si>
+    <t>15115240</t>
+  </si>
+  <si>
+    <t>RT00006479</t>
+  </si>
+  <si>
+    <t>157066809</t>
   </si>
 </sst>
 </file>
@@ -909,7 +975,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -927,14 +993,14 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1071,14 +1137,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1107,14 +1173,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1125,14 +1191,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>136</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1294,7 +1360,7 @@
         <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>135</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1307,7 +1373,7 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -1365,7 +1431,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="E27" t="s">
         <v>27</v>
@@ -1382,7 +1448,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Changes of NAM for Prod
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="166">
   <si>
     <t>Service</t>
   </si>
@@ -545,6 +545,48 @@
   </si>
   <si>
     <t>157996371</t>
+  </si>
+  <si>
+    <t>15282511</t>
+  </si>
+  <si>
+    <t>15282520</t>
+  </si>
+  <si>
+    <t>15282548</t>
+  </si>
+  <si>
+    <t>15282561</t>
+  </si>
+  <si>
+    <t>15282569</t>
+  </si>
+  <si>
+    <t>15282578</t>
+  </si>
+  <si>
+    <t>RT00006563</t>
+  </si>
+  <si>
+    <t>158940348</t>
+  </si>
+  <si>
+    <t>15282689</t>
+  </si>
+  <si>
+    <t>RT00006567</t>
+  </si>
+  <si>
+    <t>158941644</t>
+  </si>
+  <si>
+    <t>15282715</t>
+  </si>
+  <si>
+    <t>RT00006568</t>
+  </si>
+  <si>
+    <t>158941792</t>
   </si>
 </sst>
 </file>
@@ -999,7 +1041,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -1017,7 +1059,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -1161,7 +1203,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -1197,7 +1239,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
@@ -1215,7 +1257,7 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
@@ -1397,7 +1439,7 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -1455,7 +1497,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="E27" t="s">
         <v>27</v>
@@ -1472,7 +1514,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Changes of Null pointer
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1705" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="169">
   <si>
     <t>Service</t>
   </si>
@@ -587,6 +587,23 @@
   </si>
   <si>
     <t>158941792</t>
+  </si>
+  <si>
+    <t>15287826</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=122.0.6261.129)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.91', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59519}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 20ab763d4621b4c19b079e63bf171860
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>15287848</t>
   </si>
 </sst>
 </file>
@@ -1239,14 +1256,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1257,14 +1274,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>

</xml_diff>

<commit_message>
Changes of RTE OCP
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Prod.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="178">
   <si>
     <t>Service</t>
   </si>
@@ -604,6 +604,49 @@
   </si>
   <si>
     <t>15287848</t>
+  </si>
+  <si>
+    <t>15431025</t>
+  </si>
+  <si>
+    <t>15431027</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=124.0.6367.62)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL30', ip: '10.100.111.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.2'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 124.0.6367.62, chrome: {chromedriverVersion: 124.0.6367.78 (a087f2dd364d..., userDataDir: C:\Users\PARTH~1.SHA\AppDat...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:54757}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 7595c8134e3ac26d945b47a4be539aad
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>15431104</t>
+  </si>
+  <si>
+    <t>RT00006665</t>
+  </si>
+  <si>
+    <t>160628670</t>
+  </si>
+  <si>
+    <t>15431275</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome=124.0.6367.62)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL30', ip: '10.100.111.30', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.2'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 124.0.6367.62, chrome: {chromedriverVersion: 124.0.6367.78 (a087f2dd364d..., userDataDir: C:\Users\PARTH~1.SHA\AppDat...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:57094}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 7ec2368bf4d09dbd5ac05b819908f030
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>15431340</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1119,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -1220,7 +1263,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -1256,14 +1299,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1274,11 +1317,11 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
         <v>88</v>
@@ -1456,7 +1499,7 @@
         <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -1514,7 +1557,7 @@
         <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="E27" t="s">
         <v>27</v>
@@ -1531,7 +1574,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>

</xml_diff>